<commit_message>
updated specs a nd programmes
</commit_message>
<xml_diff>
--- a/Tabular programme data - AC 28092022.xlsx
+++ b/Tabular programme data - AC 28092022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmamartin\Projects\curriculumTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0021AF12-30C8-4597-9849-D4A9CC5DD5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A7075C-169E-44B0-AA3F-BFA67F1A8EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30855" yWindow="3450" windowWidth="25500" windowHeight="13560" xr2:uid="{F6BF7C93-FEFC-4CAC-964D-F381BE86B14C}"/>
+    <workbookView xWindow="30870" yWindow="720" windowWidth="25500" windowHeight="13560" activeTab="1" xr2:uid="{F6BF7C93-FEFC-4CAC-964D-F381BE86B14C}"/>
   </bookViews>
   <sheets>
     <sheet name="MILO" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3456" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="616">
   <si>
     <t>Module</t>
   </si>
@@ -1858,6 +1858,39 @@
   </si>
   <si>
     <t>route</t>
+  </si>
+  <si>
+    <t>Physiological Sciences</t>
+  </si>
+  <si>
+    <t>demonstrate an accurate understanding of how the body functions throughout the levels of organisation from chemical/molecular, through cellular to systems and organismal level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show knowledge and understanding of normal anatomy and physiology including nervous, hormonal, and other homeostatic control mechanisms </t>
+  </si>
+  <si>
+    <t>show an understanding of the impact of disease and inherent pathophysiological changes and processes on cells, tissues, and body systems</t>
+  </si>
+  <si>
+    <t>have the ability to discuss the pathophysiological processes that underpin disease and the biomedical sciences</t>
+  </si>
+  <si>
+    <t>explain the chemistry and structure of the major biological macromolecules and give detailed examples of how structure enables function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demonstrate an understanding of the molecular basis of genetics and explain some detailed examples </t>
+  </si>
+  <si>
+    <t xml:space="preserve">demonstrate critical knowledge and understanding of gene expression and how it is controlled with a detailed knowledge of specific examples and relevant experimental methods </t>
+  </si>
+  <si>
+    <t>devise and evaluate suitable experimental methods for the investigation of relevant areas of biomedical and physiological sciences</t>
+  </si>
+  <si>
+    <t>demonstrate understanding of and competence in a broad range of practical techniques and skills relevant to the biosciences in general and physiological sciences in particular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">communicate science to peers and non-scientists </t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1947,6 +1980,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2264,8 +2298,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B328" sqref="B328:B337"/>
+    <sheetView topLeftCell="A400" workbookViewId="0">
+      <selection activeCell="A391" sqref="A391:B455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,7 +2320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -5869,7 +5903,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>421</v>
       </c>
@@ -5880,7 +5914,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>421</v>
       </c>
@@ -5891,7 +5925,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>421</v>
       </c>
@@ -5902,7 +5936,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>421</v>
       </c>
@@ -5913,7 +5947,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>421</v>
       </c>
@@ -5924,7 +5958,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>421</v>
       </c>
@@ -5935,7 +5969,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>421</v>
       </c>
@@ -5946,7 +5980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>421</v>
       </c>
@@ -5957,7 +5991,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>421</v>
       </c>
@@ -5968,7 +6002,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>421</v>
       </c>
@@ -6562,7 +6596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>9</v>
       </c>
@@ -6573,7 +6607,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>9</v>
       </c>
@@ -6584,7 +6618,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>9</v>
       </c>
@@ -6595,7 +6629,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>9</v>
       </c>
@@ -6606,7 +6640,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="395" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>9</v>
       </c>
@@ -6617,7 +6651,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="396" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>9</v>
       </c>
@@ -6628,7 +6662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="397" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>9</v>
       </c>
@@ -6639,7 +6673,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>490</v>
       </c>
@@ -6650,7 +6684,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>490</v>
       </c>
@@ -6661,7 +6695,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="400" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>490</v>
       </c>
@@ -6672,7 +6706,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>490</v>
       </c>
@@ -6683,7 +6717,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>490</v>
       </c>
@@ -6694,7 +6728,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>490</v>
       </c>
@@ -6705,7 +6739,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>490</v>
       </c>
@@ -7101,7 +7135,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="440" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>530</v>
       </c>
@@ -7112,7 +7146,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="441" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
         <v>530</v>
       </c>
@@ -7123,7 +7157,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="442" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
         <v>530</v>
       </c>
@@ -7134,7 +7168,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="443" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
         <v>530</v>
       </c>
@@ -7145,7 +7179,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="444" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
         <v>530</v>
       </c>
@@ -7156,7 +7190,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="445" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
         <v>530</v>
       </c>
@@ -7167,7 +7201,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="446" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
         <v>530</v>
       </c>
@@ -7178,7 +7212,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="447" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
         <v>530</v>
       </c>
@@ -7189,7 +7223,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="448" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
         <v>530</v>
       </c>
@@ -7200,7 +7234,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="449" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
         <v>530</v>
       </c>
@@ -7211,7 +7245,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="450" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
         <v>2</v>
       </c>
@@ -7222,7 +7256,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="451" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
         <v>2</v>
       </c>
@@ -7233,7 +7267,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="452" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>2</v>
       </c>
@@ -7244,7 +7278,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="453" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
         <v>2</v>
       </c>
@@ -7255,7 +7289,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="454" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
         <v>2</v>
       </c>
@@ -7266,7 +7300,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="455" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
         <v>2</v>
       </c>
@@ -7688,7 +7722,10 @@
   <autoFilter ref="A1:D492" xr:uid="{45998FE8-448E-44A3-95CC-390E959C381D}">
     <filterColumn colId="0">
       <filters>
-        <filter val="BS21002"/>
+        <filter val="BS11001"/>
+        <filter val="BS11002"/>
+        <filter val="BS12001"/>
+        <filter val="BS12002"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A347:D360">
@@ -7703,23 +7740,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39F8078-91AC-4CD9-A02F-A295D7580066}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -7730,7 +7767,7 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
@@ -7741,7 +7778,7 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
@@ -7752,7 +7789,7 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
@@ -7763,7 +7800,7 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
@@ -7774,7 +7811,7 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -7785,7 +7822,7 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
@@ -7796,7 +7833,7 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
@@ -7807,7 +7844,7 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
@@ -7818,7 +7855,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
@@ -7829,7 +7866,7 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
@@ -7840,7 +7877,7 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
@@ -7851,7 +7888,7 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
@@ -7862,7 +7899,7 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C14" t="s">
@@ -7873,7 +7910,7 @@
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
@@ -7884,7 +7921,7 @@
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C16" t="s">
@@ -7895,7 +7932,7 @@
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C17" t="s">
@@ -7906,7 +7943,7 @@
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C18" t="s">
@@ -7917,7 +7954,7 @@
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
@@ -7928,7 +7965,7 @@
       <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
@@ -7939,7 +7976,7 @@
       <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
@@ -7950,7 +7987,7 @@
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
@@ -7961,7 +7998,7 @@
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
@@ -7972,7 +8009,7 @@
       <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C24" t="s">
@@ -7983,7 +8020,7 @@
       <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
@@ -7994,7 +8031,7 @@
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
@@ -8005,7 +8042,7 @@
       <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
@@ -8016,7 +8053,7 @@
       <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
@@ -8027,7 +8064,7 @@
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C29" t="s">
@@ -8038,7 +8075,7 @@
       <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C30" t="s">
@@ -8049,7 +8086,7 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C31" t="s">
@@ -8060,7 +8097,7 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C32" t="s">
@@ -8071,7 +8108,7 @@
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">
@@ -8082,7 +8119,7 @@
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C34" t="s">
@@ -8093,7 +8130,7 @@
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C35" t="s">
@@ -8104,7 +8141,7 @@
       <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C36" t="s">
@@ -8115,7 +8152,7 @@
       <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C37" t="s">
@@ -8126,7 +8163,7 @@
       <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C38" t="s">
@@ -8137,7 +8174,7 @@
       <c r="A39" t="s">
         <v>33</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C39" t="s">
@@ -8148,7 +8185,7 @@
       <c r="A40" t="s">
         <v>33</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C40" t="s">
@@ -8159,7 +8196,7 @@
       <c r="A41" t="s">
         <v>33</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C41" t="s">
@@ -8170,7 +8207,7 @@
       <c r="A42" t="s">
         <v>33</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C42" t="s">
@@ -8181,7 +8218,7 @@
       <c r="A43" t="s">
         <v>33</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C43" t="s">
@@ -8192,7 +8229,7 @@
       <c r="A44" t="s">
         <v>33</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C44" t="s">
@@ -8203,7 +8240,7 @@
       <c r="A45" t="s">
         <v>33</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C45" t="s">
@@ -8214,7 +8251,7 @@
       <c r="A46" t="s">
         <v>33</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C46" t="s">
@@ -8225,7 +8262,7 @@
       <c r="A47" t="s">
         <v>11</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C47" t="s">
@@ -8236,7 +8273,7 @@
       <c r="A48" t="s">
         <v>11</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C48" t="s">
@@ -8247,7 +8284,7 @@
       <c r="A49" t="s">
         <v>11</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C49" t="s">
@@ -8258,7 +8295,7 @@
       <c r="A50" t="s">
         <v>11</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C50" t="s">
@@ -8269,7 +8306,7 @@
       <c r="A51" t="s">
         <v>11</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C51" t="s">
@@ -8280,7 +8317,7 @@
       <c r="A52" t="s">
         <v>11</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C52" t="s">
@@ -8291,7 +8328,7 @@
       <c r="A53" t="s">
         <v>30</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C53" t="s">
@@ -8302,7 +8339,7 @@
       <c r="A54" t="s">
         <v>30</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C54" t="s">
@@ -8313,7 +8350,7 @@
       <c r="A55" t="s">
         <v>30</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C55" t="s">
@@ -8324,7 +8361,7 @@
       <c r="A56" t="s">
         <v>30</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C56" t="s">
@@ -8335,7 +8372,7 @@
       <c r="A57" t="s">
         <v>30</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C57" t="s">
@@ -8346,7 +8383,7 @@
       <c r="A58" t="s">
         <v>30</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C58" t="s">
@@ -8357,7 +8394,7 @@
       <c r="A59" t="s">
         <v>32</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C59" t="s">
@@ -8368,7 +8405,7 @@
       <c r="A60" t="s">
         <v>32</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C60" t="s">
@@ -8379,7 +8416,7 @@
       <c r="A61" t="s">
         <v>32</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C61" t="s">
@@ -8390,7 +8427,7 @@
       <c r="A62" t="s">
         <v>32</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C62" t="s">
@@ -8401,7 +8438,7 @@
       <c r="A63" t="s">
         <v>32</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C63" t="s">
@@ -8412,7 +8449,7 @@
       <c r="A64" t="s">
         <v>32</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C64" t="s">
@@ -8423,7 +8460,7 @@
       <c r="A65" t="s">
         <v>33</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C65" t="s">
@@ -8434,7 +8471,7 @@
       <c r="A66" t="s">
         <v>33</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C66" t="s">
@@ -8445,7 +8482,7 @@
       <c r="A67" t="s">
         <v>33</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C67" t="s">
@@ -8456,7 +8493,7 @@
       <c r="A68" t="s">
         <v>33</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C68" t="s">
@@ -8467,7 +8504,7 @@
       <c r="A69" t="s">
         <v>33</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C69" t="s">
@@ -8478,7 +8515,7 @@
       <c r="A70" t="s">
         <v>33</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C70" t="s">
@@ -8489,7 +8526,7 @@
       <c r="A71" t="s">
         <v>30</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C71" t="s">
@@ -8500,7 +8537,7 @@
       <c r="A72" t="s">
         <v>30</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C72" t="s">
@@ -8511,7 +8548,7 @@
       <c r="A73" t="s">
         <v>30</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C73" t="s">
@@ -8522,7 +8559,7 @@
       <c r="A74" t="s">
         <v>30</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C74" t="s">
@@ -8533,7 +8570,7 @@
       <c r="A75" t="s">
         <v>32</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C75" t="s">
@@ -8544,7 +8581,7 @@
       <c r="A76" t="s">
         <v>32</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C76" t="s">
@@ -8555,7 +8592,7 @@
       <c r="A77" t="s">
         <v>32</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C77" t="s">
@@ -8566,7 +8603,7 @@
       <c r="A78" t="s">
         <v>32</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C78" t="s">
@@ -8577,7 +8614,7 @@
       <c r="A79" t="s">
         <v>33</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C79" t="s">
@@ -8588,7 +8625,7 @@
       <c r="A80" t="s">
         <v>33</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C80" t="s">
@@ -8599,7 +8636,7 @@
       <c r="A81" t="s">
         <v>33</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C81" t="s">
@@ -8610,7 +8647,7 @@
       <c r="A82" t="s">
         <v>33</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C82" t="s">
@@ -8621,7 +8658,7 @@
       <c r="A83" t="s">
         <v>30</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C83" t="s">
@@ -8632,7 +8669,7 @@
       <c r="A84" t="s">
         <v>32</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C84" t="s">
@@ -8643,7 +8680,7 @@
       <c r="A85" t="s">
         <v>33</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C85" t="s">
@@ -8654,7 +8691,7 @@
       <c r="A86" t="s">
         <v>30</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C86" t="s">
@@ -8665,7 +8702,7 @@
       <c r="A87" t="s">
         <v>30</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C87" t="s">
@@ -8676,7 +8713,7 @@
       <c r="A88" t="s">
         <v>30</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C88" t="s">
@@ -8687,7 +8724,7 @@
       <c r="A89" t="s">
         <v>30</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C89" t="s">
@@ -8698,7 +8735,7 @@
       <c r="A90" t="s">
         <v>32</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C90" t="s">
@@ -8709,7 +8746,7 @@
       <c r="A91" t="s">
         <v>32</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C91" t="s">
@@ -8720,7 +8757,7 @@
       <c r="A92" t="s">
         <v>32</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C92" t="s">
@@ -8731,7 +8768,7 @@
       <c r="A93" t="s">
         <v>32</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C93" t="s">
@@ -8742,7 +8779,7 @@
       <c r="A94" t="s">
         <v>32</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C94" t="s">
@@ -8753,7 +8790,7 @@
       <c r="A95" t="s">
         <v>32</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C95" t="s">
@@ -8764,7 +8801,7 @@
       <c r="A96" t="s">
         <v>32</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C96" t="s">
@@ -8775,7 +8812,7 @@
       <c r="A97" t="s">
         <v>33</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C97" t="s">
@@ -8786,7 +8823,7 @@
       <c r="A98" t="s">
         <v>33</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C98" t="s">
@@ -8797,7 +8834,7 @@
       <c r="A99" t="s">
         <v>33</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C99" t="s">
@@ -8808,7 +8845,7 @@
       <c r="A100" t="s">
         <v>33</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C100" t="s">
@@ -8819,11 +8856,286 @@
       <c r="A101" t="s">
         <v>33</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C101" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>605</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="C102" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>605</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>607</v>
+      </c>
+      <c r="C103" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>605</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="C104" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>605</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="C105" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>605</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C106" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>605</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="C107" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>605</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="C108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>605</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="C109" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>605</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>605</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="C111" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>605</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="C112" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>605</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C113" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>605</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C114" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>605</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C115" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>605</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C116" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>605</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="C117" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>605</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C118" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>605</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>605</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C120" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>605</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>605</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C122" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>605</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C123" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>605</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C124" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>605</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C125" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>605</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C126" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>